<commit_message>
updates - anagrafica quasi completa
mancano peserico belenchia e amis
</commit_message>
<xml_diff>
--- a/Attestati Corsi di Formazione/report_gen_data/db/aziende.xlsx
+++ b/Attestati Corsi di Formazione/report_gen_data/db/aziende.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
   <si>
     <t>partita_iva</t>
   </si>
@@ -170,12 +170,18 @@
   <si>
     <t>IT00570070557</t>
   </si>
+  <si>
+    <t>ortona</t>
+  </si>
+  <si>
+    <t>Authentica S.p.A.- Ortona</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -212,14 +218,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -241,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
@@ -257,7 +255,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -451,7 +448,7 @@
   <dimension ref="A1:D14050"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -660,8 +657,18 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="B15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>

</xml_diff>

<commit_message>
commit update script vari
</commit_message>
<xml_diff>
--- a/Attestati Corsi di Formazione/report_gen_data/db/aziende.xlsx
+++ b/Attestati Corsi di Formazione/report_gen_data/db/aziende.xlsx
@@ -171,10 +171,10 @@
     <t>IT00570070557</t>
   </si>
   <si>
-    <t>ortona</t>
+    <t>Authentica S.p.A.- Ortona</t>
   </si>
   <si>
-    <t>Authentica S.p.A.- Ortona</t>
+    <t>food-and-delivery</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:D14050"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -658,10 +658,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>2</v>

</xml_diff>